<commit_message>
fix: resolve medicare discrepancy causing difference between new and old results
</commit_message>
<xml_diff>
--- a/results/07-2024/beta/inputs-07-2024.xlsx
+++ b/results/07-2024/beta/inputs-07-2024.xlsx
@@ -23338,7 +23338,7 @@
         <v>0</v>
       </c>
       <c r="AF219" t="n">
-        <v>632.926916520989</v>
+        <v>1613.48694944122</v>
       </c>
       <c r="AG219" t="n">
         <v>312.90100137919</v>
@@ -23439,7 +23439,7 @@
         <v>0</v>
       </c>
       <c r="AF220" t="n">
-        <v>637.018899068649</v>
+        <v>1633.20667325686</v>
       </c>
       <c r="AG220" t="n">
         <v>314.92396074996</v>
@@ -23540,7 +23540,7 @@
         <v>0</v>
       </c>
       <c r="AF221" t="n">
-        <v>639.346200486882</v>
+        <v>1648.15850728485</v>
       </c>
       <c r="AG221" t="n">
         <v>316.074512141074</v>
@@ -23641,7 +23641,7 @@
         <v>0</v>
       </c>
       <c r="AF222" t="n">
-        <v>641.682004528663</v>
+        <v>1663.27883267319</v>
       </c>
       <c r="AG222" t="n">
         <v>317.229266986572</v>
@@ -23742,7 +23742,7 @@
         <v>0</v>
       </c>
       <c r="AF223" t="n">
-        <v>644.026342257697</v>
+        <v>1678.56970799796</v>
       </c>
       <c r="AG223" t="n">
         <v>318.388240643464</v>
@@ -23843,7 +23843,7 @@
         <v>0</v>
       </c>
       <c r="AF224" t="n">
-        <v>646.379244851179</v>
+        <v>1694.03321764305</v>
       </c>
       <c r="AG224" t="n">
         <v>319.551448524865</v>
@@ -23944,7 +23944,7 @@
         <v>0</v>
       </c>
       <c r="AF225" t="n">
-        <v>650.109646128924</v>
+        <v>1714.25330547269</v>
       </c>
       <c r="AG225" t="n">
         <v>321.395652436698</v>
@@ -24045,7 +24045,7 @@
         <v>0</v>
       </c>
       <c r="AF226" t="n">
-        <v>653.861576398825</v>
+        <v>1734.7544638699</v>
       </c>
       <c r="AG226" t="n">
         <v>323.250499667734</v>

</xml_diff>

<commit_message>
Run the FIM with the old order
Unfortunately, the projections do not match. Will have to investigate.
</commit_message>
<xml_diff>
--- a/results/07-2024/beta/inputs-07-2024.xlsx
+++ b/results/07-2024/beta/inputs-07-2024.xlsx
@@ -23254,43 +23254,43 @@
         <v>0</v>
       </c>
       <c r="D219" t="n">
-        <v>0.00631342210315755</v>
+        <v>0.00814832810809674</v>
       </c>
       <c r="E219" t="n">
-        <v>0.00809347092440249</v>
+        <v>0.00991870914463755</v>
       </c>
       <c r="F219" t="n">
-        <v>0.00809347092440249</v>
+        <v>0.00991870914463755</v>
       </c>
       <c r="G219" t="n">
-        <v>0.00809347092440249</v>
+        <v>0.00991870914463755</v>
       </c>
       <c r="H219" t="n">
-        <v>0.00600439160454336</v>
+        <v>0.00784098294506985</v>
       </c>
       <c r="I219" t="n">
         <v>0.00514477147642989</v>
       </c>
       <c r="J219" t="n">
-        <v>28642.997691315</v>
+        <v>28658.5</v>
       </c>
       <c r="K219" t="n">
-        <v>1825.69462457217</v>
+        <v>1863.8</v>
       </c>
       <c r="L219" t="n">
-        <v>418.030017283248</v>
+        <v>433.054109</v>
       </c>
       <c r="M219" t="n">
         <v>77.7072857142857</v>
       </c>
       <c r="N219" t="n">
-        <v>3143.68342111664</v>
+        <v>3137.4</v>
       </c>
       <c r="O219" t="n">
-        <v>4464.98832083441</v>
+        <v>4439</v>
       </c>
       <c r="P219" t="n">
-        <v>2315.22358241816</v>
+        <v>2328.3</v>
       </c>
       <c r="Q219" t="n">
         <v>464.974716755204</v>
@@ -23302,7 +23302,7 @@
         <v>172.78949768486</v>
       </c>
       <c r="T219" t="n">
-        <v>2053.43233333333</v>
+        <v>2070.499</v>
       </c>
       <c r="U219" t="n">
         <v>199.524772892058</v>
@@ -23314,13 +23314,13 @@
         <v>0</v>
       </c>
       <c r="X219" t="n">
-        <v>0</v>
+        <v>0.300000000000001</v>
       </c>
       <c r="Y219" t="n">
         <v>22.5</v>
       </c>
       <c r="Z219" t="n">
-        <v>95.135</v>
+        <v>92.635</v>
       </c>
       <c r="AA219" t="n">
         <v>1.365</v>
@@ -23338,10 +23338,10 @@
         <v>0</v>
       </c>
       <c r="AF219" t="n">
-        <v>1613.48694944122</v>
+        <v>1606.2</v>
       </c>
       <c r="AG219" t="n">
-        <v>312.90100137919</v>
+        <v>319.7</v>
       </c>
     </row>
     <row r="220">
@@ -23355,16 +23355,16 @@
         <v>0</v>
       </c>
       <c r="D220" t="n">
-        <v>0.00680665617807996</v>
+        <v>0.00631637071565883</v>
       </c>
       <c r="E220" t="n">
-        <v>0.00612458852946784</v>
+        <v>0.00563330429941056</v>
       </c>
       <c r="F220" t="n">
-        <v>0.00612458852946784</v>
+        <v>0.00563330429941056</v>
       </c>
       <c r="G220" t="n">
-        <v>0.00612458852946784</v>
+        <v>0.00563330429941056</v>
       </c>
       <c r="H220" t="n">
         <v>0.00557191872235663</v>
@@ -23373,25 +23373,25 @@
         <v>0.0051977939134229</v>
       </c>
       <c r="J220" t="n">
-        <v>28953.2297859252</v>
+        <v>28968.9</v>
       </c>
       <c r="K220" t="n">
-        <v>1824.70794990839</v>
+        <v>1862.79273174517</v>
       </c>
       <c r="L220" t="n">
-        <v>422.510222582441</v>
+        <v>437.682352782907</v>
       </c>
       <c r="M220" t="n">
         <v>77.7072857142857</v>
       </c>
       <c r="N220" t="n">
-        <v>3173.05560450168</v>
+        <v>3166.71347588412</v>
       </c>
       <c r="O220" t="n">
-        <v>4497.01044575673</v>
+        <v>4488.43810791123</v>
       </c>
       <c r="P220" t="n">
-        <v>2347.06775494829</v>
+        <v>2365.66523074806</v>
       </c>
       <c r="Q220" t="n">
         <v>476.424608245003</v>
@@ -23403,7 +23403,7 @@
         <v>175.488406763014</v>
       </c>
       <c r="T220" t="n">
-        <v>2060.36566666667</v>
+        <v>2077.43233333333</v>
       </c>
       <c r="U220" t="n">
         <v>202.804265449591</v>
@@ -23421,7 +23421,7 @@
         <v>22.5</v>
       </c>
       <c r="Z220" t="n">
-        <v>95.135</v>
+        <v>92.635</v>
       </c>
       <c r="AA220" t="n">
         <v>1.365</v>
@@ -23439,10 +23439,10 @@
         <v>0</v>
       </c>
       <c r="AF220" t="n">
-        <v>1633.20667325686</v>
+        <v>1632.88132683418</v>
       </c>
       <c r="AG220" t="n">
-        <v>314.92396074996</v>
+        <v>322.260664845667</v>
       </c>
     </row>
     <row r="221">
@@ -23456,16 +23456,16 @@
         <v>0</v>
       </c>
       <c r="D221" t="n">
-        <v>0.00629989728491442</v>
+        <v>0.00580887002259489</v>
       </c>
       <c r="E221" t="n">
-        <v>0.00583217133289549</v>
+        <v>0.00534045807802097</v>
       </c>
       <c r="F221" t="n">
-        <v>0.00583217133289549</v>
+        <v>0.00534045807802097</v>
       </c>
       <c r="G221" t="n">
-        <v>0.00583217133289549</v>
+        <v>0.00534045807802097</v>
       </c>
       <c r="H221" t="n">
         <v>0.00508257870201945</v>
@@ -23474,25 +23474,25 @@
         <v>0.00524986184574083</v>
       </c>
       <c r="J221" t="n">
-        <v>29240.674213792</v>
+        <v>29256.5</v>
       </c>
       <c r="K221" t="n">
-        <v>1842.72297444865</v>
+        <v>1881.18376071914</v>
       </c>
       <c r="L221" t="n">
-        <v>427.281525681758</v>
+        <v>442.603153049303</v>
       </c>
       <c r="M221" t="n">
         <v>79.3012857142857</v>
       </c>
       <c r="N221" t="n">
-        <v>3202.05401447002</v>
+        <v>3195.65392542925</v>
       </c>
       <c r="O221" t="n">
-        <v>4528.04269697862</v>
+        <v>4537.15803906129</v>
       </c>
       <c r="P221" t="n">
-        <v>2370.91028523945</v>
+        <v>2389.58107566087</v>
       </c>
       <c r="Q221" t="n">
         <v>485.992461156107</v>
@@ -23504,7 +23504,7 @@
         <v>176.811168794724</v>
       </c>
       <c r="T221" t="n">
-        <v>2068.827</v>
+        <v>2085.89366666667</v>
       </c>
       <c r="U221" t="n">
         <v>206.137661446175</v>
@@ -23522,7 +23522,7 @@
         <v>22.5</v>
       </c>
       <c r="Z221" t="n">
-        <v>102.234</v>
+        <v>99.734</v>
       </c>
       <c r="AA221" t="n">
         <v>-0.901</v>
@@ -23540,10 +23540,10 @@
         <v>0</v>
       </c>
       <c r="AF221" t="n">
-        <v>1648.15850728485</v>
+        <v>1648.41368264403</v>
       </c>
       <c r="AG221" t="n">
-        <v>316.074512141074</v>
+        <v>323.696248231545</v>
       </c>
     </row>
     <row r="222">
@@ -23557,16 +23557,16 @@
         <v>0</v>
       </c>
       <c r="D222" t="n">
-        <v>0.00603935957081481</v>
+        <v>0.00554795034724531</v>
       </c>
       <c r="E222" t="n">
-        <v>0.00639382889171092</v>
+        <v>0.00590293924064178</v>
       </c>
       <c r="F222" t="n">
-        <v>0.00639382889171092</v>
+        <v>0.00590293924064178</v>
       </c>
       <c r="G222" t="n">
-        <v>0.00639382889171092</v>
+        <v>0.00590293924064178</v>
       </c>
       <c r="H222" t="n">
         <v>0.0054050287894607</v>
@@ -23575,25 +23575,25 @@
         <v>0.00530534068053212</v>
       </c>
       <c r="J222" t="n">
-        <v>29540.6118800049</v>
+        <v>29556.6</v>
       </c>
       <c r="K222" t="n">
-        <v>1864.46175450651</v>
+        <v>1903.37626636961</v>
       </c>
       <c r="L222" t="n">
-        <v>410.471077</v>
+        <v>425.943674590989</v>
       </c>
       <c r="M222" t="n">
         <v>79.3012857142857</v>
       </c>
       <c r="N222" t="n">
-        <v>3230.02358731572</v>
+        <v>3223.56759423466</v>
       </c>
       <c r="O222" t="n">
-        <v>4601.45619287391</v>
+        <v>4610.85968628637</v>
       </c>
       <c r="P222" t="n">
-        <v>2395.48839414195</v>
+        <v>2414.22849555631</v>
       </c>
       <c r="Q222" t="n">
         <v>495.752461592221</v>
@@ -23605,7 +23605,7 @@
         <v>178.430514241616</v>
       </c>
       <c r="T222" t="n">
-        <v>2110.60894127433</v>
+        <v>2127.619844211</v>
       </c>
       <c r="U222" t="n">
         <v>209.525846866667</v>
@@ -23623,7 +23623,7 @@
         <v>22.5</v>
       </c>
       <c r="Z222" t="n">
-        <v>102.234</v>
+        <v>99.734</v>
       </c>
       <c r="AA222" t="n">
         <v>-0.901</v>
@@ -23641,10 +23641,10 @@
         <v>0</v>
       </c>
       <c r="AF222" t="n">
-        <v>1663.27883267319</v>
+        <v>1664.11988720118</v>
       </c>
       <c r="AG222" t="n">
-        <v>317.229266986572</v>
+        <v>325.138226749943</v>
       </c>
     </row>
     <row r="223">
@@ -23658,16 +23658,16 @@
         <v>0</v>
       </c>
       <c r="D223" t="n">
-        <v>0.00587526180714026</v>
+        <v>0.00538361180457825</v>
       </c>
       <c r="E223" t="n">
-        <v>0.00631345033117214</v>
+        <v>0.00582244292745138</v>
       </c>
       <c r="F223" t="n">
-        <v>0.00631345033117214</v>
+        <v>0.00582244292745138</v>
       </c>
       <c r="G223" t="n">
-        <v>0.00631345033117214</v>
+        <v>0.00582244292745138</v>
       </c>
       <c r="H223" t="n">
         <v>0.00535108244542615</v>
@@ -23676,25 +23676,25 @@
         <v>0.0053207417791068</v>
       </c>
       <c r="J223" t="n">
-        <v>29847.845597412</v>
+        <v>29864</v>
       </c>
       <c r="K223" t="n">
-        <v>1887.06419677237</v>
+        <v>1926.45046033837</v>
       </c>
       <c r="L223" t="n">
-        <v>405.818404114578</v>
+        <v>421.4434595</v>
       </c>
       <c r="M223" t="n">
         <v>75.2292857142857</v>
       </c>
       <c r="N223" t="n">
-        <v>3258.12732619472</v>
+        <v>3251.6151609097</v>
       </c>
       <c r="O223" t="n">
-        <v>4633.18149018033</v>
+        <v>4642.55171794178</v>
       </c>
       <c r="P223" t="n">
-        <v>2420.0058245704</v>
+        <v>2438.81450200309</v>
       </c>
       <c r="Q223" t="n">
         <v>505.708468378488</v>
@@ -23706,7 +23706,7 @@
         <v>180.043928020205</v>
       </c>
       <c r="T223" t="n">
-        <v>2117.54227460767</v>
+        <v>2134.55317754433</v>
       </c>
       <c r="U223" t="n">
         <v>212.969722258429</v>
@@ -23724,7 +23724,7 @@
         <v>22.5</v>
       </c>
       <c r="Z223" t="n">
-        <v>95.212</v>
+        <v>92.712</v>
       </c>
       <c r="AA223" t="n">
         <v>-0.901</v>
@@ -23742,10 +23742,10 @@
         <v>0</v>
       </c>
       <c r="AF223" t="n">
-        <v>1678.56970799796</v>
+        <v>1680.00204124785</v>
       </c>
       <c r="AG223" t="n">
-        <v>318.388240643464</v>
+        <v>326.586628889433</v>
       </c>
     </row>
     <row r="224">
@@ -23759,16 +23759,16 @@
         <v>0</v>
       </c>
       <c r="D224" t="n">
-        <v>0.00581704113714143</v>
+        <v>0.00532530567014544</v>
       </c>
       <c r="E224" t="n">
-        <v>0.00621564390753804</v>
+        <v>0.00572449316892887</v>
       </c>
       <c r="F224" t="n">
-        <v>0.00621564390753804</v>
+        <v>0.00572449316892887</v>
       </c>
       <c r="G224" t="n">
-        <v>0.00621564390753804</v>
+        <v>0.00572449316892887</v>
       </c>
       <c r="H224" t="n">
         <v>0.00513746411938887</v>
@@ -23777,25 +23777,25 @@
         <v>0.00534438472662901</v>
       </c>
       <c r="J224" t="n">
-        <v>30149.0825604129</v>
+        <v>30165.4</v>
       </c>
       <c r="K224" t="n">
-        <v>1910.23633527942</v>
+        <v>1950.10624108514</v>
       </c>
       <c r="L224" t="n">
-        <v>408.367496285738</v>
+        <v>424.146511694223</v>
       </c>
       <c r="M224" t="n">
         <v>75.2292857142857</v>
       </c>
       <c r="N224" t="n">
-        <v>3285.21298207225</v>
+        <v>3278.64667947144</v>
       </c>
       <c r="O224" t="n">
-        <v>4665.15298287264</v>
+        <v>4674.48863793118</v>
       </c>
       <c r="P224" t="n">
-        <v>2443.56426350959</v>
+        <v>2462.44011672197</v>
       </c>
       <c r="Q224" t="n">
         <v>515.864417835356</v>
@@ -23807,7 +23807,7 @@
         <v>181.070106636733</v>
       </c>
       <c r="T224" t="n">
-        <v>2124.475607941</v>
+        <v>2141.48651087767</v>
       </c>
       <c r="U224" t="n">
         <v>216.470202970687</v>
@@ -23825,7 +23825,7 @@
         <v>22.5</v>
       </c>
       <c r="Z224" t="n">
-        <v>96.212</v>
+        <v>93.712</v>
       </c>
       <c r="AA224" t="n">
         <v>-0.901</v>
@@ -23843,10 +23843,10 @@
         <v>0</v>
       </c>
       <c r="AF224" t="n">
-        <v>1694.03321764305</v>
+        <v>1696.06227169245</v>
       </c>
       <c r="AG224" t="n">
-        <v>319.551448524865</v>
+        <v>328.041483265495</v>
       </c>
     </row>
     <row r="225">
@@ -23860,16 +23860,16 @@
         <v>0</v>
       </c>
       <c r="D225" t="n">
-        <v>0.00583138024509955</v>
+        <v>0.00533966582888934</v>
       </c>
       <c r="E225" t="n">
-        <v>0.00616214863410014</v>
+        <v>0.00567091947478038</v>
       </c>
       <c r="F225" t="n">
-        <v>0.00616214863410014</v>
+        <v>0.00567091947478038</v>
       </c>
       <c r="G225" t="n">
-        <v>0.00616214863410014</v>
+        <v>0.00567091947478038</v>
       </c>
       <c r="H225" t="n">
         <v>0.00499022561961571</v>
@@ -23878,25 +23878,25 @@
         <v>0.00535891413284784</v>
       </c>
       <c r="J225" t="n">
-        <v>30434.9278537715</v>
+        <v>30451.4</v>
       </c>
       <c r="K225" t="n">
-        <v>1923.87666798075</v>
+        <v>1964.03127090479</v>
       </c>
       <c r="L225" t="n">
-        <v>407.056006781028</v>
+        <v>422.990499243275</v>
       </c>
       <c r="M225" t="n">
         <v>75.2292857142857</v>
       </c>
       <c r="N225" t="n">
-        <v>3312.27542171367</v>
+        <v>3305.65502820041</v>
       </c>
       <c r="O225" t="n">
-        <v>4697.37284077022</v>
+        <v>4706.67259288094</v>
       </c>
       <c r="P225" t="n">
-        <v>2466.81066529387</v>
+        <v>2485.75498407887</v>
       </c>
       <c r="Q225" t="n">
         <v>526.224325334891</v>
@@ -23908,7 +23908,7 @@
         <v>181.159081661288</v>
       </c>
       <c r="T225" t="n">
-        <v>2115.16994127433</v>
+        <v>2132.180844211</v>
       </c>
       <c r="U225" t="n">
         <v>220.02821939782</v>
@@ -23926,7 +23926,7 @@
         <v>22.5</v>
       </c>
       <c r="Z225" t="n">
-        <v>101.551</v>
+        <v>99.051</v>
       </c>
       <c r="AA225" t="n">
         <v>-2.15</v>
@@ -23944,10 +23944,10 @@
         <v>0</v>
       </c>
       <c r="AF225" t="n">
-        <v>1714.25330547269</v>
+        <v>1716.89000384285</v>
       </c>
       <c r="AG225" t="n">
-        <v>321.395652436698</v>
+        <v>330.193673423702</v>
       </c>
     </row>
     <row r="226">
@@ -23961,16 +23961,16 @@
         <v>0</v>
       </c>
       <c r="D226" t="n">
-        <v>0.00445436582290237</v>
+        <v>0.00396062435642164</v>
       </c>
       <c r="E226" t="n">
-        <v>0.00617427290467454</v>
+        <v>0.0056830615202379</v>
       </c>
       <c r="F226" t="n">
-        <v>0.00617427290467454</v>
+        <v>0.0056830615202379</v>
       </c>
       <c r="G226" t="n">
-        <v>0.00617427290467454</v>
+        <v>0.0056830615202379</v>
       </c>
       <c r="H226" t="n">
         <v>0.00490394615593148</v>
@@ -23979,25 +23979,25 @@
         <v>0.00533462036210497</v>
       </c>
       <c r="J226" t="n">
-        <v>30700.9838575899</v>
+        <v>30717.6</v>
       </c>
       <c r="K226" t="n">
-        <v>1936.19570222756</v>
+        <v>1976.60742450692</v>
       </c>
       <c r="L226" t="n">
-        <v>409.781722</v>
+        <v>425.873223494629</v>
       </c>
       <c r="M226" t="n">
         <v>75.2292857142857</v>
       </c>
       <c r="N226" t="n">
-        <v>3340.46531464436</v>
+        <v>3333.78857672717</v>
       </c>
       <c r="O226" t="n">
-        <v>4780.1184210202</v>
+        <v>4789.764743375</v>
       </c>
       <c r="P226" t="n">
-        <v>2487.60294797483</v>
+        <v>2506.61206147365</v>
       </c>
       <c r="Q226" t="n">
         <v>536.792286888337</v>
@@ -24009,7 +24009,7 @@
         <v>180.364238108601</v>
       </c>
       <c r="T226" t="n">
-        <v>2159.15720553131</v>
+        <v>2176.11106217219</v>
       </c>
       <c r="U226" t="n">
         <v>223.644717226652</v>
@@ -24027,7 +24027,7 @@
         <v>22.5</v>
       </c>
       <c r="Z226" t="n">
-        <v>100.401</v>
+        <v>97.901</v>
       </c>
       <c r="AA226" t="n">
         <v>0</v>
@@ -24045,10 +24045,10 @@
         <v>0</v>
       </c>
       <c r="AF226" t="n">
-        <v>1734.7544638699</v>
+        <v>1738.00706068685</v>
       </c>
       <c r="AG226" t="n">
-        <v>323.250499667734</v>
+        <v>332.359983510982</v>
       </c>
     </row>
     <row r="227">
@@ -24062,25 +24062,25 @@
         <v>0</v>
       </c>
       <c r="D227" t="n">
-        <v>0.00467044581501486</v>
+        <v>0</v>
       </c>
       <c r="E227" t="n">
-        <v>0.00620433826657418</v>
+        <v>0</v>
       </c>
       <c r="F227" t="n">
-        <v>0.00620433826657418</v>
+        <v>0</v>
       </c>
       <c r="G227" t="n">
-        <v>0.00620433826657418</v>
+        <v>0</v>
       </c>
       <c r="H227" t="n">
-        <v>0.00484384269748661</v>
+        <v>0</v>
       </c>
       <c r="I227" t="n">
         <v>0.00530631319568364</v>
       </c>
       <c r="J227" t="n">
-        <v>30970.8378058654</v>
+        <v>30987.6</v>
       </c>
       <c r="K227" t="n">
         <v>0</v>
@@ -24181,7 +24181,7 @@
         <v>0.00527407883226472</v>
       </c>
       <c r="J228" t="n">
-        <v>31251.7857497923</v>
+        <v>31268.7</v>
       </c>
       <c r="K228" t="n">
         <v>0</v>
@@ -24282,7 +24282,7 @@
         <v>0.00523379729860385</v>
       </c>
       <c r="J229" t="n">
-        <v>31535.7320709222</v>
+        <v>31552.8</v>
       </c>
       <c r="K229" t="n">
         <v>0</v>
@@ -24383,7 +24383,7 @@
         <v>0.00522327514825061</v>
       </c>
       <c r="J230" t="n">
-        <v>31815.5806098747</v>
+        <v>31832.8</v>
       </c>
       <c r="K230" t="n">
         <v>0</v>
@@ -24484,7 +24484,7 @@
         <v>0.00515037171705424</v>
       </c>
       <c r="J231" t="n">
-        <v>32092.8305552511</v>
+        <v>32110.2</v>
       </c>
       <c r="K231" t="n">
         <v>0</v>
@@ -24585,7 +24585,7 @@
         <v>0.00510328671531268</v>
       </c>
       <c r="J232" t="n">
-        <v>32373.3787155509</v>
+        <v>32390.9</v>
       </c>
       <c r="K232" t="n">
         <v>0</v>
@@ -24686,7 +24686,7 @@
         <v>0.00506502170135303</v>
       </c>
       <c r="J233" t="n">
-        <v>32657.6248744012</v>
+        <v>32675.3</v>
       </c>
       <c r="K233" t="n">
         <v>0</v>
@@ -24787,7 +24787,7 @@
         <v>0.00501081648038282</v>
       </c>
       <c r="J234" t="n">
-        <v>32946.1687072425</v>
+        <v>32964</v>
       </c>
       <c r="K234" t="n">
         <v>0</v>
@@ -24888,7 +24888,7 @@
         <v>0.00502660062373872</v>
       </c>
       <c r="J235" t="n">
-        <v>33241.6088076508</v>
+        <v>33259.6</v>
       </c>
       <c r="K235" t="n">
         <v>0</v>
@@ -24989,7 +24989,7 @@
         <v>0.00501362928348925</v>
       </c>
       <c r="J236" t="n">
-        <v>33543.4454460924</v>
+        <v>33561.6</v>
       </c>
       <c r="K236" t="n">
         <v>0</v>
@@ -25090,7 +25090,7 @@
         <v>0.00500072649779626</v>
       </c>
       <c r="J237" t="n">
-        <v>33851.5786766604</v>
+        <v>33869.9</v>
       </c>
       <c r="K237" t="n">
         <v>0</v>
@@ -25191,7 +25191,7 @@
         <v>0.00497584366453419</v>
       </c>
       <c r="J238" t="n">
-        <v>34165.1089861938</v>
+        <v>34183.6</v>
       </c>
       <c r="K238" t="n">
         <v>0</v>
@@ -25292,7 +25292,7 @@
         <v>0.00496719175837779</v>
       </c>
       <c r="J239" t="n">
-        <v>34484.1363205996</v>
+        <v>34502.8</v>
       </c>
       <c r="K239" t="n">
         <v>0</v>
@@ -25393,7 +25393,7 @@
         <v>0.00492673519295383</v>
       </c>
       <c r="J240" t="n">
-        <v>34807.8611126235</v>
+        <v>34826.7</v>
       </c>
       <c r="K240" t="n">
         <v>0</v>
@@ -25494,7 +25494,7 @@
         <v>0.00488279704341488</v>
       </c>
       <c r="J241" t="n">
-        <v>35135.3838491046</v>
+        <v>35154.4</v>
       </c>
       <c r="K241" t="n">
         <v>0</v>
@@ -25595,7 +25595,7 @@
         <v>0.00482756991313527</v>
       </c>
       <c r="J242" t="n">
-        <v>35465.9049627888</v>
+        <v>35485.1</v>
       </c>
       <c r="K242" t="n">
         <v>0</v>
@@ -25696,7 +25696,7 @@
         <v>0.0047847827449996</v>
       </c>
       <c r="J243" t="n">
-        <v>35799.9241832099</v>
+        <v>35819.3</v>
       </c>
       <c r="K243" t="n">
         <v>0</v>
@@ -25797,7 +25797,7 @@
         <v>0.00475029738109622</v>
       </c>
       <c r="J244" t="n">
-        <v>36137.5414562746</v>
+        <v>36157.1</v>
       </c>
       <c r="K244" t="n">
         <v>0</v>
@@ -25898,7 +25898,7 @@
         <v>0.00472007545910125</v>
       </c>
       <c r="J245" t="n">
-        <v>36478.6568360763</v>
+        <v>36498.4</v>
       </c>
       <c r="K245" t="n">
         <v>0</v>
@@ -25999,7 +25999,7 @@
         <v>0.00468244739007639</v>
       </c>
       <c r="J246" t="n">
-        <v>36822.8705389878</v>
+        <v>36842.8</v>
       </c>
       <c r="K246" t="n">
         <v>0</v>
@@ -26100,7 +26100,7 @@
         <v>0.00465677886260774</v>
       </c>
       <c r="J247" t="n">
-        <v>37170.2825109159</v>
+        <v>37190.4</v>
       </c>
       <c r="K247" t="n">
         <v>0</v>
@@ -26201,7 +26201,7 @@
         <v>0.00462371106398929</v>
       </c>
       <c r="J248" t="n">
-        <v>37521.0926436741</v>
+        <v>37541.4</v>
       </c>
       <c r="K248" t="n">
         <v>0</v>
@@ -26302,7 +26302,7 @@
         <v>0.00459481083552404</v>
       </c>
       <c r="J249" t="n">
-        <v>37874.3014781947</v>
+        <v>37894.8</v>
       </c>
       <c r="K249" t="n">
         <v>0</v>
@@ -26403,7 +26403,7 @@
         <v>0.00456241751240172</v>
       </c>
       <c r="J250" t="n">
-        <v>38229.9090144779</v>
+        <v>38250.6</v>
       </c>
       <c r="K250" t="n">
         <v>0</v>
@@ -26504,7 +26504,7 @@
         <v>0.00454169639722291</v>
       </c>
       <c r="J251" t="n">
-        <v>38588.5149279641</v>
+        <v>38609.4</v>
       </c>
       <c r="K251" t="n">
         <v>0</v>
@@ -26605,7 +26605,7 @@
         <v>0.00450988792928486</v>
       </c>
       <c r="J252" t="n">
-        <v>38950.3191104668</v>
+        <v>38971.4</v>
       </c>
       <c r="K252" t="n">
         <v>0</v>
@@ -26706,7 +26706,7 @@
         <v>0.00448215742174929</v>
       </c>
       <c r="J253" t="n">
-        <v>39314.9217783591</v>
+        <v>39336.2</v>
       </c>
       <c r="K253" t="n">
         <v>0</v>
@@ -26807,7 +26807,7 @@
         <v>0.00445843265792623</v>
       </c>
       <c r="J254" t="n">
-        <v>39682.2229857342</v>
+        <v>39703.7</v>
       </c>
       <c r="K254" t="n">
         <v>0</v>
@@ -26908,7 +26908,7 @@
         <v>0.00443122698635778</v>
       </c>
       <c r="J255" t="n">
-        <v>40052.4226244056</v>
+        <v>40074.1</v>
       </c>
       <c r="K255" t="n">
         <v>0</v>
@@ -27009,7 +27009,7 @@
         <v>0.00441167784045593</v>
       </c>
       <c r="J256" t="n">
-        <v>40425.7205861868</v>
+        <v>40447.6</v>
       </c>
       <c r="K256" t="n">
         <v>0</v>
@@ -27110,7 +27110,7 @@
         <v>0.00439230042599803</v>
       </c>
       <c r="J257" t="n">
-        <v>40802.2168169845</v>
+        <v>40824.3</v>
       </c>
       <c r="K257" t="n">
         <v>0</v>
@@ -27211,7 +27211,7 @@
         <v>0.00437675198161469</v>
       </c>
       <c r="J258" t="n">
-        <v>41182.2111545192</v>
+        <v>41204.5</v>
       </c>
       <c r="K258" t="n">
         <v>0</v>
@@ -27312,7 +27312,7 @@
         <v>0.00435767949923127</v>
       </c>
       <c r="J259" t="n">
-        <v>41565.5037069773</v>
+        <v>41588</v>
       </c>
       <c r="K259" t="n">
         <v>0</v>
@@ -27413,7 +27413,7 @@
         <v>0.00433514478295249</v>
       </c>
       <c r="J260" t="n">
-        <v>41952.2943661723</v>
+        <v>41975</v>
       </c>
       <c r="K260" t="n">
         <v>0</v>

</xml_diff>

<commit_message>
feat: correct forecast sheet error in taxes
</commit_message>
<xml_diff>
--- a/results/07-2024/beta/inputs-07-2024.xlsx
+++ b/results/07-2024/beta/inputs-07-2024.xlsx
@@ -23700,7 +23700,7 @@
         <v>505.708468378488</v>
       </c>
       <c r="R223" t="n">
-        <v>142.305433390167</v>
+        <v>142.305433390168</v>
       </c>
       <c r="S223" t="n">
         <v>180.043928020205</v>
@@ -23724,7 +23724,7 @@
         <v>22.5</v>
       </c>
       <c r="Z223" t="n">
-        <v>92.712</v>
+        <v>91.712</v>
       </c>
       <c r="AA223" t="n">
         <v>-0.901</v>
@@ -23825,7 +23825,7 @@
         <v>22.5</v>
       </c>
       <c r="Z224" t="n">
-        <v>93.712</v>
+        <v>91.712</v>
       </c>
       <c r="AA224" t="n">
         <v>-0.901</v>
@@ -23899,7 +23899,7 @@
         <v>2485.75498407887</v>
       </c>
       <c r="Q225" t="n">
-        <v>526.224325334891</v>
+        <v>514.561789254755</v>
       </c>
       <c r="R225" t="n">
         <v>149.344899197861</v>
@@ -23926,7 +23926,7 @@
         <v>22.5</v>
       </c>
       <c r="Z225" t="n">
-        <v>99.051</v>
+        <v>96.051</v>
       </c>
       <c r="AA225" t="n">
         <v>-2.15</v>
@@ -24000,7 +24000,7 @@
         <v>2506.61206147365</v>
       </c>
       <c r="Q226" t="n">
-        <v>536.792286888337</v>
+        <v>513.262449990416</v>
       </c>
       <c r="R226" t="n">
         <v>151.584820456769</v>
@@ -24027,7 +24027,7 @@
         <v>22.5</v>
       </c>
       <c r="Z226" t="n">
-        <v>97.901</v>
+        <v>93.901</v>
       </c>
       <c r="AA226" t="n">
         <v>0</v>
@@ -24083,37 +24083,37 @@
         <v>30955.9187647644</v>
       </c>
       <c r="K227" t="n">
-        <v>0</v>
+        <v>1991.53866628079</v>
       </c>
       <c r="L227" t="n">
-        <v>0</v>
+        <v>425.9813524</v>
       </c>
       <c r="M227" t="n">
-        <v>0</v>
+        <v>75.2292857142857</v>
       </c>
       <c r="N227" t="n">
-        <v>0</v>
+        <v>3361.53574377562</v>
       </c>
       <c r="O227" t="n">
-        <v>0</v>
+        <v>4822.70071085096</v>
       </c>
       <c r="P227" t="n">
-        <v>0</v>
+        <v>2528.31878066128</v>
       </c>
       <c r="Q227" t="n">
-        <v>0</v>
+        <v>511.966391736364</v>
       </c>
       <c r="R227" t="n">
-        <v>0</v>
+        <v>152.319073482388</v>
       </c>
       <c r="S227" t="n">
-        <v>0</v>
+        <v>180.233741405921</v>
       </c>
       <c r="T227" t="n">
-        <v>0</v>
+        <v>2182.31639550552</v>
       </c>
       <c r="U227" t="n">
-        <v>0</v>
+        <v>227.320657687805</v>
       </c>
       <c r="V227" t="n">
         <v>0</v>
@@ -24125,10 +24125,10 @@
         <v>0</v>
       </c>
       <c r="Y227" t="n">
-        <v>0</v>
+        <v>22.5</v>
       </c>
       <c r="Z227" t="n">
-        <v>0</v>
+        <v>93.901</v>
       </c>
       <c r="AA227" t="n">
         <v>0</v>
@@ -24140,16 +24140,16 @@
         <v>0</v>
       </c>
       <c r="AD227" t="n">
-        <v>0</v>
+        <v>2.71754</v>
       </c>
       <c r="AE227" t="n">
         <v>0</v>
       </c>
       <c r="AF227" t="n">
-        <v>0</v>
+        <v>1759.41774352578</v>
       </c>
       <c r="AG227" t="n">
-        <v>0</v>
+        <v>334.540506164317</v>
       </c>
     </row>
     <row r="228">

</xml_diff>

<commit_message>
data: run the FIM with corrected deflators
</commit_message>
<xml_diff>
--- a/results/07-2024/beta/inputs-07-2024.xlsx
+++ b/results/07-2024/beta/inputs-07-2024.xlsx
@@ -24062,19 +24062,19 @@
         <v>0</v>
       </c>
       <c r="D227" t="n">
-        <v>0</v>
+        <v>0.00417702316823587</v>
       </c>
       <c r="E227" t="n">
-        <v>0</v>
+        <v>0.00571317095599766</v>
       </c>
       <c r="F227" t="n">
-        <v>0</v>
+        <v>0.00571317095599766</v>
       </c>
       <c r="G227" t="n">
-        <v>0</v>
+        <v>0.00571317095599766</v>
       </c>
       <c r="H227" t="n">
-        <v>0</v>
+        <v>0.00484384269748661</v>
       </c>
       <c r="I227" t="n">
         <v>0.00530631319568364</v>

</xml_diff>